<commit_message>
Downloaing files - last edits 2018
</commit_message>
<xml_diff>
--- a/users and keys.xlsx
+++ b/users and keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewisspurgin/Documents/Teaching/PopGenBerlin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{72F979A1-593A-904D-8FB8-A2C507651463}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3520F762-CCB3-874A-9C92-FF11ED64D249}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="1580" windowWidth="19900" windowHeight="12740" xr2:uid="{91A6C049-0161-4F51-B2A5-23E096B56351}"/>
   </bookViews>
@@ -369,9 +369,6 @@
     <t>eelizo@udel.edu</t>
   </si>
   <si>
-    <t>nathalie.isabel@canada.ca</t>
-  </si>
-  <si>
     <t>m.lisette.delgado@dal.ca</t>
   </si>
   <si>
@@ -421,6 +418,9 @@
   </si>
   <si>
     <t>c33.pem</t>
+  </si>
+  <si>
+    <t>nisabel65@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB60074E-F500-453D-BA17-063026CAA746}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1014,7 +1014,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1022,11 +1022,11 @@
         <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>103</v>
@@ -1193,8 +1193,8 @@
       <c r="D21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>114</v>
+      <c r="E21" s="9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1209,7 +1209,7 @@
         <v>22</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1224,7 +1224,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1254,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1269,7 +1269,7 @@
         <v>26</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1284,7 +1284,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1299,7 +1299,7 @@
         <v>28</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1314,7 +1314,7 @@
         <v>61</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1329,7 +1329,7 @@
         <v>62</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1344,7 +1344,7 @@
         <v>63</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
         <v>64</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1374,7 +1374,7 @@
         <v>65</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1397,20 +1397,20 @@
     <hyperlink ref="E19" r:id="rId16" display="javascript:void(0);" xr:uid="{A5C3A7DA-7920-4AAB-B4B3-7A6B2AB22311}"/>
     <hyperlink ref="E15" r:id="rId17" display="javascript:void(0);" xr:uid="{C8778296-BDAA-463E-B86C-B776B5FAE3B5}"/>
     <hyperlink ref="E20" r:id="rId18" display="javascript:void(0);" xr:uid="{20BFCDB1-9AFA-43D0-AF71-55CB984C7F85}"/>
-    <hyperlink ref="E21" r:id="rId19" display="javascript:void(0);" xr:uid="{8FB82BE6-81C3-4D8C-84C4-ABA6F568F3AD}"/>
-    <hyperlink ref="E23" r:id="rId20" display="javascript:void(0);" xr:uid="{81087445-4A2E-4F08-8D22-688DAE5E1847}"/>
-    <hyperlink ref="E25" r:id="rId21" display="javascript:void(0);" xr:uid="{22737607-9C2C-4E8F-9CFA-6438E1BC198C}"/>
-    <hyperlink ref="E26" r:id="rId22" display="javascript:void(0);" xr:uid="{68CEA505-260B-4B6A-A980-79EDB5A432BE}"/>
-    <hyperlink ref="E27" r:id="rId23" display="javascript:void(0);" xr:uid="{FD4B39D7-F477-438E-8ECB-B98612B72258}"/>
-    <hyperlink ref="E28" r:id="rId24" display="javascript:void(0);" xr:uid="{F13D42C2-0F70-4CB5-98A1-F08699FCB2F9}"/>
-    <hyperlink ref="E30" r:id="rId25" display="javascript:void(0);" xr:uid="{C4E26C3E-EC3C-40CA-828C-C0AB81064932}"/>
-    <hyperlink ref="E31" r:id="rId26" display="javascript:void(0);" xr:uid="{A8C7A46F-AD07-46C0-8009-D3090998EFB1}"/>
-    <hyperlink ref="E29" r:id="rId27" xr:uid="{847D8619-2500-4B4F-AAD0-F306553D4F2D}"/>
-    <hyperlink ref="E32" r:id="rId28" xr:uid="{BF6B62E0-D69B-4E33-A37E-E8B0B8E79D6E}"/>
-    <hyperlink ref="E33" r:id="rId29" display="javascript:void(0);" xr:uid="{6CC99446-A70B-49B6-B267-858B767C9315}"/>
-    <hyperlink ref="E5" r:id="rId30" display="javascript:void(0);" xr:uid="{07CB1B4A-6528-4A19-A1F3-D38499DB77CC}"/>
-    <hyperlink ref="E22" r:id="rId31" xr:uid="{9E0D9AF0-458A-3E4C-B999-45DD1E6016E7}"/>
-    <hyperlink ref="E24" r:id="rId32" xr:uid="{D1263EE8-786A-4742-A66E-1487504420B2}"/>
+    <hyperlink ref="E23" r:id="rId19" display="javascript:void(0);" xr:uid="{81087445-4A2E-4F08-8D22-688DAE5E1847}"/>
+    <hyperlink ref="E25" r:id="rId20" display="javascript:void(0);" xr:uid="{22737607-9C2C-4E8F-9CFA-6438E1BC198C}"/>
+    <hyperlink ref="E26" r:id="rId21" display="javascript:void(0);" xr:uid="{68CEA505-260B-4B6A-A980-79EDB5A432BE}"/>
+    <hyperlink ref="E27" r:id="rId22" display="javascript:void(0);" xr:uid="{FD4B39D7-F477-438E-8ECB-B98612B72258}"/>
+    <hyperlink ref="E28" r:id="rId23" display="javascript:void(0);" xr:uid="{F13D42C2-0F70-4CB5-98A1-F08699FCB2F9}"/>
+    <hyperlink ref="E30" r:id="rId24" display="javascript:void(0);" xr:uid="{C4E26C3E-EC3C-40CA-828C-C0AB81064932}"/>
+    <hyperlink ref="E31" r:id="rId25" display="javascript:void(0);" xr:uid="{A8C7A46F-AD07-46C0-8009-D3090998EFB1}"/>
+    <hyperlink ref="E29" r:id="rId26" xr:uid="{847D8619-2500-4B4F-AAD0-F306553D4F2D}"/>
+    <hyperlink ref="E32" r:id="rId27" xr:uid="{BF6B62E0-D69B-4E33-A37E-E8B0B8E79D6E}"/>
+    <hyperlink ref="E33" r:id="rId28" display="javascript:void(0);" xr:uid="{6CC99446-A70B-49B6-B267-858B767C9315}"/>
+    <hyperlink ref="E5" r:id="rId29" display="javascript:void(0);" xr:uid="{07CB1B4A-6528-4A19-A1F3-D38499DB77CC}"/>
+    <hyperlink ref="E22" r:id="rId30" xr:uid="{9E0D9AF0-458A-3E4C-B999-45DD1E6016E7}"/>
+    <hyperlink ref="E24" r:id="rId31" xr:uid="{D1263EE8-786A-4742-A66E-1487504420B2}"/>
+    <hyperlink ref="E21" r:id="rId32" display="mailto:nisabel65@gmail.com" xr:uid="{E19A737F-960F-2743-A904-8F6CF3476D99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>

</xml_diff>